<commit_message>
Fill some missing columns according to the suggestion in the group at 3/5/2020.
</commit_message>
<xml_diff>
--- a/TUMLM/TUMLM_acc_info.xlsx
+++ b/TUMLM/TUMLM_acc_info.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t xml:space="preserve">Technology University Account Setting</t>
   </si>
@@ -34,15 +34,45 @@
     <t xml:space="preserve">Username</t>
   </si>
   <si>
-    <t xml:space="preserve">change password</t>
+    <t xml:space="preserve">Change Password</t>
   </si>
   <si>
     <t xml:space="preserve">Name</t>
   </si>
   <si>
+    <t xml:space="preserve">Birth Of Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Student ID Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NRC Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Major </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Father Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mother Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Race </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Religion</t>
+  </si>
+  <si>
     <t xml:space="preserve">Email Address</t>
   </si>
   <si>
+    <t xml:space="preserve">First Year Roll</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Second Year To Final Year Roll</t>
+  </si>
+  <si>
     <t xml:space="preserve">Street </t>
   </si>
   <si>
@@ -67,7 +97,7 @@
     <t xml:space="preserve">Mobile Phone</t>
   </si>
   <si>
-    <t xml:space="preserve">emergency phone</t>
+    <t xml:space="preserve">Emergency Phone</t>
   </si>
 </sst>
 </file>
@@ -82,6 +112,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -103,17 +134,20 @@
       <sz val="13"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -158,7 +192,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -167,7 +201,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -175,8 +209,12 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -196,25 +234,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ3"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.07"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.98"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="5" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.26"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="9" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="12.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="12.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="16.44"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="14" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="6" style="1" width="12.98"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="17" min="13" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="13.26"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="20" min="19" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="12.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="12.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="16.44"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="24" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -233,9 +273,18 @@
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
-      <c r="AMJ1" s="0"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -253,53 +302,93 @@
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="4"/>
+      <c r="W2" s="4"/>
     </row>
-    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+    <row r="3" s="5" customFormat="true" ht="35.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M3" s="5" t="s">
         <v>15</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="S3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="T3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="U3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="V3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="W3" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A1:W1"/>
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:M2"/>
+    <mergeCell ref="C2:W2"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>